<commit_message>
ZM Sanity run for BE & BS
</commit_message>
<xml_diff>
--- a/Excels/ZM.xlsx
+++ b/Excels/ZM.xlsx
@@ -2872,9 +2872,6 @@
     <t>973099626</t>
   </si>
   <si>
-    <t>VGFyZ2V0QDA9</t>
-  </si>
-  <si>
     <t>Row9</t>
   </si>
   <si>
@@ -3066,6 +3063,9 @@
   </si>
   <si>
     <t>SmFuQDIwMjE</t>
+  </si>
+  <si>
+    <t>VGFyZ2V0QDA0</t>
   </si>
 </sst>
 </file>
@@ -5059,7 +5059,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5358,7 +5358,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5459,7 +5459,7 @@
         <v>2388192</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>894</v>
@@ -5488,7 +5488,7 @@
         <v>23103239</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>912</v>
+        <v>975</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>895</v>
@@ -6295,7 +6295,7 @@
         <v>125</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6415,16 +6415,16 @@
         <v>30</v>
       </c>
       <c r="J1" s="44" t="s">
+        <v>912</v>
+      </c>
+      <c r="K1" s="44" t="s">
         <v>913</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="L1" s="18" t="s">
         <v>914</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>915</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -6432,7 +6432,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>32</v>
@@ -6471,7 +6471,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -6495,7 +6495,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>35</v>
@@ -6647,22 +6647,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
+        <v>918</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>919</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
+        <v>969</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>920</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>970</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>921</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>922</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>923</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -6674,22 +6674,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
+        <v>923</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>924</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="18" t="s">
         <v>926</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="E11" s="18" t="s">
         <v>927</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="18" t="s">
         <v>928</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>929</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -6701,28 +6701,28 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
+        <v>929</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>930</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>931</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="18" t="s">
         <v>932</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="E12" s="18" t="s">
         <v>933</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="18" t="s">
         <v>934</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="18" t="s">
         <v>935</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="H12" s="18" t="s">
         <v>936</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>937</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -6732,19 +6732,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>937</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>938</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>939</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="D13" s="18" t="s">
         <v>940</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="E13" s="18" t="s">
         <v>941</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>942</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -6757,7 +6757,7 @@
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>160</v>
@@ -6769,22 +6769,22 @@
         <v>42</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F14" s="44" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="44" t="s">
+        <v>944</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>945</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>946</v>
       </c>
       <c r="I14" s="44" t="s">
         <v>61</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="K14" s="44" t="s">
         <v>48</v>
@@ -6794,7 +6794,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>37</v>
@@ -6806,13 +6806,13 @@
         <v>40</v>
       </c>
       <c r="E15" s="44" t="s">
+        <v>948</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>916</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>949</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>917</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>950</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>42</v>
@@ -6825,16 +6825,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
+        <v>950</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>951</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>952</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="18" t="s">
         <v>953</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>954</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>139</v>
@@ -6850,19 +6850,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
+        <v>954</v>
+      </c>
+      <c r="B17" s="44" t="s">
         <v>955</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="C17" s="44" t="s">
         <v>956</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="D17" s="44" t="s">
         <v>957</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="E17" s="44" t="s">
         <v>958</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>959</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -6875,13 +6875,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
+        <v>959</v>
+      </c>
+      <c r="B18" s="44" t="s">
         <v>960</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="C18" s="44" t="s">
         <v>961</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>962</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>35</v>
@@ -6898,43 +6898,43 @@
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="44" t="s">
+        <v>963</v>
+      </c>
+      <c r="E19" s="44" t="s">
         <v>964</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="F19" s="44" t="s">
         <v>965</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="G19" s="44" t="s">
         <v>966</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>967</v>
       </c>
       <c r="H19" s="44" t="s">
         <v>34</v>
       </c>
       <c r="I19" s="51" t="s">
+        <v>970</v>
+      </c>
+      <c r="J19" s="51" t="s">
         <v>971</v>
       </c>
-      <c r="J19" s="51" t="s">
+      <c r="K19" s="51" t="s">
         <v>972</v>
-      </c>
-      <c r="K19" s="51" t="s">
-        <v>973</v>
       </c>
       <c r="L19" s="44" t="s">
         <v>35</v>
       </c>
       <c r="M19" s="44" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dashboard Revamp Changes made related to widget
</commit_message>
<xml_diff>
--- a/Excels/ZM.xlsx
+++ b/Excels/ZM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4246" uniqueCount="978">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3066,6 +3066,12 @@
   </si>
   <si>
     <t>VGFyZ2V0QDA0</t>
+  </si>
+  <si>
+    <t>HLR Code Detail</t>
+  </si>
+  <si>
+    <t>Service Details</t>
   </si>
 </sst>
 </file>
@@ -5357,8 +5363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6380,8 +6386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6427,12 +6433,12 @@
         <v>915</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>968</v>
+        <v>858</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>32</v>
@@ -6880,14 +6886,18 @@
       <c r="B18" s="44" t="s">
         <v>960</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>961</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>139</v>
+      </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
@@ -6939,7 +6949,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Auth tab and Transfer to Queue
</commit_message>
<xml_diff>
--- a/Excels/ZM.xlsx
+++ b/Excels/ZM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4251" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233" uniqueCount="982">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -2857,9 +2857,6 @@
     <t>RGVhdGhub3RlQDEyMw</t>
   </si>
   <si>
-    <t>No Authenication policy statement configured</t>
-  </si>
-  <si>
     <t>8926001030998120000</t>
   </si>
   <si>
@@ -3084,6 +3081,9 @@
   </si>
   <si>
     <t>Test Data-Prod</t>
+  </si>
+  <si>
+    <t>no authentication policy statement configured</t>
   </si>
 </sst>
 </file>
@@ -3158,7 +3158,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3201,8 +3201,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3342,6 +3348,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA9D08E"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFA9D08E"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA9D08E"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFA9D08E"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA9D08E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3352,7 +3382,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
@@ -3526,6 +3556,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5432,10 +5466,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="18" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>909</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -5456,7 +5490,7 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
@@ -5467,10 +5501,10 @@
         <v>119</v>
       </c>
       <c r="P2" s="78" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -5478,7 +5512,7 @@
         <v>2388192</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>894</v>
@@ -5491,7 +5525,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
@@ -5507,7 +5541,7 @@
         <v>23103239</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>895</v>
@@ -5520,7 +5554,7 @@
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
@@ -5549,7 +5583,7 @@
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
@@ -5709,7 +5743,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5740,8 +5774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5795,7 +5829,7 @@
         <v>221</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>907</v>
+        <v>981</v>
       </c>
       <c r="C2" s="76">
         <v>3</v>
@@ -5832,7 +5866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -5861,10 +5895,10 @@
         <v>145</v>
       </c>
       <c r="H1" s="79" t="s">
+        <v>979</v>
+      </c>
+      <c r="I1" s="79" t="s">
         <v>980</v>
-      </c>
-      <c r="I1" s="79" t="s">
-        <v>981</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -5880,13 +5914,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>977</v>
+      </c>
+      <c r="H3" t="s">
         <v>978</v>
       </c>
-      <c r="H3" t="s">
-        <v>979</v>
-      </c>
       <c r="I3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -6312,8 +6346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6331,7 +6365,7 @@
         <v>125</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6347,10 +6381,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -6451,16 +6485,16 @@
         <v>30</v>
       </c>
       <c r="J1" s="44" t="s">
+        <v>911</v>
+      </c>
+      <c r="K1" s="44" t="s">
         <v>912</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="L1" s="18" t="s">
         <v>913</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>914</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6507,7 +6541,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -6531,7 +6565,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>35</v>
@@ -6683,22 +6717,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
+        <v>917</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>918</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
+        <v>968</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>919</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>969</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>920</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>921</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>922</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -6710,22 +6744,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>923</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>924</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="18" t="s">
         <v>925</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="E11" s="18" t="s">
         <v>926</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="18" t="s">
         <v>927</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>928</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -6737,28 +6771,28 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
+        <v>928</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>929</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>930</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="18" t="s">
         <v>931</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="E12" s="18" t="s">
         <v>932</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="18" t="s">
         <v>933</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="18" t="s">
         <v>934</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="H12" s="18" t="s">
         <v>935</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>936</v>
       </c>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
@@ -6768,19 +6802,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>937</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>938</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="D13" s="18" t="s">
         <v>939</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="E13" s="18" t="s">
         <v>940</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>941</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -6793,7 +6827,7 @@
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>160</v>
@@ -6805,22 +6839,22 @@
         <v>42</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F14" s="44" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="44" t="s">
+        <v>943</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>944</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>945</v>
       </c>
       <c r="I14" s="44" t="s">
         <v>61</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="K14" s="44" t="s">
         <v>48</v>
@@ -6830,7 +6864,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>37</v>
@@ -6842,13 +6876,13 @@
         <v>40</v>
       </c>
       <c r="E15" s="44" t="s">
+        <v>947</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>915</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>948</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>916</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>949</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>42</v>
@@ -6861,16 +6895,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
+        <v>949</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>950</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="C16" s="18" t="s">
         <v>951</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="D16" s="18" t="s">
         <v>952</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>953</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>139</v>
@@ -6886,19 +6920,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
+        <v>953</v>
+      </c>
+      <c r="B17" s="44" t="s">
         <v>954</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="C17" s="44" t="s">
         <v>955</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="D17" s="44" t="s">
         <v>956</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="E17" s="44" t="s">
         <v>957</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>958</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -6911,19 +6945,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
+        <v>958</v>
+      </c>
+      <c r="B18" s="44" t="s">
         <v>959</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="C18" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>960</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>977</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>961</v>
-      </c>
       <c r="E18" s="19" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>139</v>
@@ -6938,43 +6972,43 @@
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="44" t="s">
+        <v>962</v>
+      </c>
+      <c r="E19" s="44" t="s">
         <v>963</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="F19" s="44" t="s">
         <v>964</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="G19" s="44" t="s">
         <v>965</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>966</v>
       </c>
       <c r="H19" s="44" t="s">
         <v>34</v>
       </c>
       <c r="I19" s="51" t="s">
+        <v>969</v>
+      </c>
+      <c r="J19" s="51" t="s">
         <v>970</v>
       </c>
-      <c r="J19" s="51" t="s">
+      <c r="K19" s="51" t="s">
         <v>971</v>
-      </c>
-      <c r="K19" s="51" t="s">
-        <v>972</v>
       </c>
       <c r="L19" s="44" t="s">
         <v>35</v>
       </c>
       <c r="M19" s="44" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>
@@ -6988,8 +7022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BA3" sqref="BA3"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BJ5" sqref="BJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7173,48 +7207,21 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="51" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>645</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>645</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>834</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>853</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>854</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="I2" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="53" t="s">
-        <v>856</v>
-      </c>
-      <c r="L2" s="53" t="s">
-        <v>857</v>
-      </c>
-      <c r="M2" s="53" t="s">
-        <v>854</v>
-      </c>
-      <c r="N2" s="53" t="s">
-        <v>209</v>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
+        <v>403</v>
+      </c>
+      <c r="B2" s="81" t="s">
+        <v>767</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>835</v>
       </c>
       <c r="AV2" t="s">
         <v>883</v>
@@ -7229,48 +7236,21 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>835</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>853</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>854</v>
-      </c>
-      <c r="H3" s="53" t="s">
-        <v>209</v>
-      </c>
-      <c r="I3" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="53" t="s">
-        <v>856</v>
-      </c>
-      <c r="L3" s="53" t="s">
-        <v>857</v>
-      </c>
-      <c r="M3" s="53" t="s">
-        <v>854</v>
-      </c>
-      <c r="N3" s="53" t="s">
-        <v>209</v>
+      <c r="C3" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>834</v>
       </c>
       <c r="AV3" t="s">
         <v>883</v>
@@ -7300,7 +7280,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7328,38 +7308,38 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>447</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>448</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>448</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="82" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>449</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>450</v>
+      <c r="B2" s="83" t="s">
+        <v>415</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>627</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>627</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Widget Tag Issue Test
</commit_message>
<xml_diff>
--- a/Excels/ZM.xlsx
+++ b/Excels/ZM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
@@ -31,7 +31,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4233" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4239" uniqueCount="988">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3085,11 +3085,30 @@
   <si>
     <t>no authentication policy statement configured</t>
   </si>
+  <si>
+    <t>200321000122</t>
+  </si>
+  <si>
+    <t>200321000123</t>
+  </si>
+  <si>
+    <t>210321000125</t>
+  </si>
+  <si>
+    <t>210321000126</t>
+  </si>
+  <si>
+    <t>210321000128</t>
+  </si>
+  <si>
+    <t>210321000129</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5112,7 +5131,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5416,7 +5435,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -5780,7 +5799,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.25">
@@ -6352,9 +6371,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="26.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="27.7109375" collapsed="true"/>
+    <col min="3" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7235,6 +7254,9 @@
       <c r="BE2" s="25" t="s">
         <v>198</v>
       </c>
+      <c r="BG2" t="s">
+        <v>986</v>
+      </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="82" t="s">
@@ -7263,6 +7285,9 @@
       </c>
       <c r="BE3" s="25" t="s">
         <v>198</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -7285,7 +7310,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -7362,7 +7387,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="74"/>
+    <col min="1" max="1" style="74" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
@@ -20790,7 +20815,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>